<commit_message>
Fix test config file column names to match code expectations
ISSUE: Test config had 'parameter' and 'value' columns but code expects
'Setting' and 'Value' (capitalized) per load_config_sheet() function.

FIX: Regenerated test_segment_config.xlsx with correct column names:
- parameter → Setting
- value → Value

Now matches the format expected by config_utils.R
</commit_message>
<xml_diff>
--- a/modules/segment/test_data/test_segment_config.xlsx
+++ b/modules/segment/test_data/test_segment_config.xlsx
@@ -424,12 +424,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>parameter</t>
+          <t>Setting</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>value</t>
+          <t>Value</t>
         </is>
       </c>
     </row>

</xml_diff>